<commit_message>
Decreased probability of fetal death before 4 weeks from conception and modified anlaysis function to calculate SEs for truth. Identified some errors in the data generation and analysis files.
</commit_message>
<xml_diff>
--- a/Scenario 1.xlsx
+++ b/Scenario 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaselatour/Multiple_outcomes_pregnancy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D450F29-F105-9D4B-ACD3-1A3FB5DA9B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680449F3-3CE4-1448-A10C-2CC02741DBAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="4" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
+    <workbookView xWindow="32320" yWindow="820" windowWidth="28800" windowHeight="16220" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
   </bookViews>
   <sheets>
     <sheet name="Phase1" sheetId="6" r:id="rId1"/>
@@ -394,7 +394,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -423,12 +423,6 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -456,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -467,7 +461,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -899,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0633E7-A8AC-2448-856C-6ACF1A963AAB}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -933,14 +926,14 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
         <f>1-C2-B2</f>
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -951,14 +944,14 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
         <f>1-C3-B3</f>
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -969,14 +962,14 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
         <f>1-C4-B4</f>
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -987,14 +980,14 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
         <f>1-C5-B5</f>
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1678,7 +1671,7 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D39" sqref="D39:D41"/>
+      <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1715,14 +1708,14 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
         <f>1-D2-C2</f>
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1733,14 +1726,14 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E5" si="0">1-D3-C3</f>
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1751,14 +1744,14 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1769,14 +1762,14 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2430,7 +2423,7 @@
         <f>0.8*Phase1!B39</f>
         <v>2.8000000000000003E-4</v>
       </c>
-      <c r="D39" s="8">
+      <c r="D39">
         <f>1.05*Phase1!C39</f>
         <v>0.73499999999999999</v>
       </c>
@@ -2450,7 +2443,7 @@
         <f>0.8*Phase1!B40</f>
         <v>3.3600000000000004E-4</v>
       </c>
-      <c r="D40" s="8">
+      <c r="D40">
         <f>1.05*Phase1!C40</f>
         <v>0.73499999999999999</v>
       </c>
@@ -2470,7 +2463,7 @@
         <f>0.8*Phase1!B41</f>
         <v>4.8799999999999999E-4</v>
       </c>
-      <c r="D41" s="8">
+      <c r="D41">
         <f>1.05*Phase1!C41</f>
         <v>0.73499999999999999</v>
       </c>
@@ -2543,7 +2536,7 @@
       <c r="F1" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" t="s">
         <v>0</v>
       </c>
       <c r="H1" t="s">
@@ -3148,7 +3141,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638C0E0C-D6E1-F442-8735-4FA62BD9AC1D}">
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
@@ -5211,6 +5204,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006F311363ECB49C45BE6A1ABA8AA4E3C9" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bcab42b681813b96043c0b869577973d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7962a6ab-b148-4fb3-9b24-47c6fd02e414" xmlns:ns3="78c38721-2d96-443e-bd32-82c62d4eed8a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b36b52368701cf0b88ba8d42da5a3441" ns2:_="" ns3:_="">
     <xsd:import namespace="7962a6ab-b148-4fb3-9b24-47c6fd02e414"/>
@@ -5435,16 +5437,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC4DEEE-E4C1-4BDA-9F3A-10B42714F00A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDB1F164-DDC9-4622-8588-A1C1F4AFED79}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5461,12 +5462,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC4DEEE-E4C1-4BDA-9F3A-10B42714F00A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>